<commit_message>
handling errors in loading excel file with consumption
</commit_message>
<xml_diff>
--- a/resources/Esempio_input_consumi_multienergetico.xlsx
+++ b/resources/Esempio_input_consumi_multienergetico.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimoneMazzieri\Desktop\Enea\enea-simulatore-cer\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RaffaellaAssogna\Desktop\REVOLT\ENEA\enea-simulatore-cer\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75E1363C-8B59-4122-81EC-343906DEC165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E06790-7BB4-4CAB-B2A0-6817734EFBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{92639A9F-4A77-45D5-A503-8B06D589BB7E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{92639A9F-4A77-45D5-A503-8B06D589BB7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -38,23 +38,23 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Consumi energetici kWh</t>
-  </si>
-  <si>
     <t>Consumi Termici (J)</t>
   </si>
   <si>
     <t>Consumi Frigoriferi (kWh)</t>
   </si>
   <si>
-    <t>Ore</t>
+    <t>Consumi elettrici (kWh)</t>
+  </si>
+  <si>
+    <t>Ora</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +64,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -91,10 +99,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -437,7 +448,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,13 +464,13 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -492,7 +503,7 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -70671,7 +70682,7 @@
       <c r="D8777" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="tTgNFAD+i4ePQsshDVbkZ5XwNybZkhSXlF77pyyHv5KvtBe7jmD1/9OH+Qi8Vqw26oScQ3rB9EoQy4OcctFkgg==" saltValue="wIBkCV3J8jTOEoEGoEYtQw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Errore inserimento dati" error="Il valore deve essere &gt;= 0" sqref="B2:D8777" xr:uid="{624166E2-10D7-4880-AB49-FCE5A4AFFC49}">
       <formula1>0</formula1>
@@ -70877,6 +70888,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="e3188f7c-f259-4833-880e-f6051f1ef813">
@@ -70885,15 +70905,6 @@
     <TaxCatchAll xmlns="c145ff50-5f07-4080-8332-af404e1983a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -70916,6 +70927,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{172124E8-5AA1-44BE-A8A9-9CE3BCBD422E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C764A327-5314-40C0-9F7C-471864663B51}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -70924,12 +70943,4 @@
     <ds:schemaRef ds:uri="c145ff50-5f07-4080-8332-af404e1983a5"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{172124E8-5AA1-44BE-A8A9-9CE3BCBD422E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated file excel and control on number of rows
</commit_message>
<xml_diff>
--- a/resources/Esempio_input_consumi_multienergetico.xlsx
+++ b/resources/Esempio_input_consumi_multienergetico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RaffaellaAssogna\Desktop\REVOLT\ENEA\enea-simulatore-cer\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E06790-7BB4-4CAB-B2A0-6817734EFBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AE3454-7EEB-465A-80EC-96999125C929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{92639A9F-4A77-45D5-A503-8B06D589BB7E}"/>
   </bookViews>
@@ -445,10 +445,10 @@
   <dimension ref="A1:D8777"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8657" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="B8768" sqref="B8768"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -70554,135 +70554,87 @@
       <c r="D8761" s="2"/>
     </row>
     <row r="8762" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8762" s="1">
-        <v>8761</v>
-      </c>
       <c r="B8762" s="2"/>
       <c r="C8762" s="2"/>
       <c r="D8762" s="2"/>
     </row>
     <row r="8763" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8763" s="1">
-        <v>8762</v>
-      </c>
       <c r="B8763" s="2"/>
       <c r="C8763" s="2"/>
       <c r="D8763" s="2"/>
     </row>
     <row r="8764" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8764" s="1">
-        <v>8763</v>
-      </c>
       <c r="B8764" s="2"/>
       <c r="C8764" s="2"/>
       <c r="D8764" s="2"/>
     </row>
     <row r="8765" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8765" s="1">
-        <v>8764</v>
-      </c>
       <c r="B8765" s="2"/>
       <c r="C8765" s="2"/>
       <c r="D8765" s="2"/>
     </row>
     <row r="8766" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8766" s="1">
-        <v>8765</v>
-      </c>
       <c r="B8766" s="2"/>
       <c r="C8766" s="2"/>
       <c r="D8766" s="2"/>
     </row>
     <row r="8767" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8767" s="1">
-        <v>8766</v>
-      </c>
       <c r="B8767" s="2"/>
       <c r="C8767" s="2"/>
       <c r="D8767" s="2"/>
     </row>
     <row r="8768" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8768" s="1">
-        <v>8767</v>
-      </c>
       <c r="B8768" s="2"/>
       <c r="C8768" s="2"/>
       <c r="D8768" s="2"/>
     </row>
-    <row r="8769" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8769" s="1">
-        <v>8768</v>
-      </c>
+    <row r="8769" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8769" s="2"/>
       <c r="C8769" s="2"/>
       <c r="D8769" s="2"/>
     </row>
-    <row r="8770" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8770" s="1">
-        <v>8769</v>
-      </c>
+    <row r="8770" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8770" s="2"/>
       <c r="C8770" s="2"/>
       <c r="D8770" s="2"/>
     </row>
-    <row r="8771" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8771" s="1">
-        <v>8770</v>
-      </c>
+    <row r="8771" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8771" s="2"/>
       <c r="C8771" s="2"/>
       <c r="D8771" s="2"/>
     </row>
-    <row r="8772" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8772" s="1">
-        <v>8771</v>
-      </c>
+    <row r="8772" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8772" s="2"/>
       <c r="C8772" s="2"/>
       <c r="D8772" s="2"/>
     </row>
-    <row r="8773" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8773" s="1">
-        <v>8772</v>
-      </c>
+    <row r="8773" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8773" s="2"/>
       <c r="C8773" s="2"/>
       <c r="D8773" s="2"/>
     </row>
-    <row r="8774" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8774" s="1">
-        <v>8773</v>
-      </c>
+    <row r="8774" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8774" s="2"/>
       <c r="C8774" s="2"/>
       <c r="D8774" s="2"/>
     </row>
-    <row r="8775" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8775" s="1">
-        <v>8774</v>
-      </c>
+    <row r="8775" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8775" s="2"/>
       <c r="C8775" s="2"/>
       <c r="D8775" s="2"/>
     </row>
-    <row r="8776" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8776" s="1">
-        <v>8775</v>
-      </c>
+    <row r="8776" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8776" s="2"/>
       <c r="C8776" s="2"/>
       <c r="D8776" s="2"/>
     </row>
-    <row r="8777" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8777" s="1">
-        <v>8776</v>
-      </c>
+    <row r="8777" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8777" s="2"/>
       <c r="C8777" s="2"/>
       <c r="D8777" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="tTgNFAD+i4ePQsshDVbkZ5XwNybZkhSXlF77pyyHv5KvtBe7jmD1/9OH+Qi8Vqw26oScQ3rB9EoQy4OcctFkgg==" saltValue="wIBkCV3J8jTOEoEGoEYtQw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Errore inserimento dati" error="Il valore deve essere &gt;= 0" sqref="B2:D8777" xr:uid="{624166E2-10D7-4880-AB49-FCE5A4AFFC49}">
       <formula1>0</formula1>
@@ -70888,15 +70840,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="e3188f7c-f259-4833-880e-f6051f1ef813">
@@ -70905,6 +70848,15 @@
     <TaxCatchAll xmlns="c145ff50-5f07-4080-8332-af404e1983a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -70927,14 +70879,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{172124E8-5AA1-44BE-A8A9-9CE3BCBD422E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C764A327-5314-40C0-9F7C-471864663B51}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -70943,4 +70887,12 @@
     <ds:schemaRef ds:uri="c145ff50-5f07-4080-8332-af404e1983a5"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{172124E8-5AA1-44BE-A8A9-9CE3BCBD422E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
wip : controller multivector
</commit_message>
<xml_diff>
--- a/resources/Esempio_input_consumi_multienergetico.xlsx
+++ b/resources/Esempio_input_consumi_multienergetico.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RaffaellaAssogna\Desktop\REVOLT\ENEA\enea-simulatore-cer\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimoneMazzieri\Desktop\Enea\enea-simulatore-cer\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AE3454-7EEB-465A-80EC-96999125C929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C995282-86BB-4378-9CB5-23B57DCF8FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{92639A9F-4A77-45D5-A503-8B06D589BB7E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{92639A9F-4A77-45D5-A503-8B06D589BB7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -38,16 +38,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Consumi Termici (J)</t>
-  </si>
-  <si>
     <t>Consumi Frigoriferi (kWh)</t>
   </si>
   <si>
-    <t>Consumi elettrici (kWh)</t>
+    <t>Ora</t>
   </si>
   <si>
-    <t>Ora</t>
+    <t>Consumi Termici (kWh)</t>
+  </si>
+  <si>
+    <t>Consumi Elettrici (kWh)</t>
   </si>
 </sst>
 </file>
@@ -445,32 +445,32 @@
   <dimension ref="A1:D8777"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8657" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B8768" sqref="B8768"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -551,7 +551,6 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -70636,7 +70635,7 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Errore inserimento dati" error="Il valore deve essere &gt;= 0" sqref="B2:D8777" xr:uid="{624166E2-10D7-4880-AB49-FCE5A4AFFC49}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Errore inserimento dati" error="Il valore deve essere &gt;= 0" sqref="B12:D8777 B11:C11 B2:D10" xr:uid="{624166E2-10D7-4880-AB49-FCE5A4AFFC49}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>